<commit_message>
modifico caso de prueba 01
</commit_message>
<xml_diff>
--- a/CP01.xlsx
+++ b/CP01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>WEB
 GITHUB</t>
@@ -59,6 +59,9 @@
     <t>Tener una cuenta de E-mail</t>
   </si>
   <si>
+    <t>usuario: carlos123</t>
+  </si>
+  <si>
     <t>1-Ingresar a la web https://github.com/
 2-Seleccionar el boton SIGN UP
 3-Ingresar email en el campo "Email"
@@ -71,7 +74,7 @@
     <t>Deberia permitir el acceso a la web</t>
   </si>
   <si>
-    <t>usuario: carlos@hotmail.com</t>
+    <t>email: carlos@hotmail.com</t>
   </si>
   <si>
     <t>contraseña: carlos123</t>
@@ -82,12 +85,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -130,12 +133,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF3C78D8"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -147,6 +144,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -154,8 +159,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,6 +176,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
@@ -178,21 +192,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,9 +236,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,37 +281,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
@@ -275,24 +288,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,13 +340,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,55 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,79 +508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,26 +518,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -636,9 +633,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -663,19 +658,19 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,7 +694,46 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,30 +753,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -751,181 +761,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -965,23 +949,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1255,7 +1236,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1270,7 +1251,7 @@
     <col min="8" max="8" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="13.5" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1259,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" ht="13.5" spans="1:3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -1325,24 +1306,26 @@
       <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" spans="1:8">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
       <c r="D5" s="20"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="23" t="s">
-        <v>16</v>
+      <c r="F5" s="17" t="s">
+        <v>17</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="20"/>
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:8">
@@ -1351,10 +1334,10 @@
       <c r="C6" s="21"/>
       <c r="D6" s="20"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="23" t="s">
-        <v>17</v>
+      <c r="F6" s="17" t="s">
+        <v>18</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="20"/>
     </row>
     <row r="7" ht="41" customHeight="1" spans="1:8">
@@ -1363,8 +1346,8 @@
       <c r="C7" s="21"/>
       <c r="D7" s="20"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="20"/>
     </row>
     <row r="8" ht="54" customHeight="1" spans="3:3">
@@ -1394,118 +1377,118 @@
     <row r="16" spans="3:3">
       <c r="C16" s="4"/>
     </row>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
+    <row r="17" ht="12.75"/>
+    <row r="18" ht="12.75"/>
+    <row r="19" ht="12.75"/>
+    <row r="20" ht="12.75"/>
+    <row r="21" ht="12.75"/>
+    <row r="22" ht="12.75"/>
+    <row r="23" ht="12.75"/>
+    <row r="24" ht="12.75"/>
+    <row r="25" ht="12.75"/>
+    <row r="26" ht="12.75"/>
+    <row r="27" ht="12.75"/>
+    <row r="28" ht="12.75"/>
+    <row r="29" ht="12.75"/>
+    <row r="30" ht="12.75"/>
+    <row r="31" ht="12.75"/>
+    <row r="32" ht="12.75"/>
+    <row r="33" ht="12.75"/>
+    <row r="34" ht="12.75"/>
+    <row r="35" ht="12.75"/>
+    <row r="36" ht="12.75"/>
     <row r="37" ht="12" customHeight="1"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
+    <row r="38" ht="12.75"/>
+    <row r="39" ht="12.75"/>
+    <row r="40" ht="12.75"/>
+    <row r="41" ht="12.75"/>
     <row r="42" ht="24.75" customHeight="1"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
+    <row r="43" ht="12.75"/>
+    <row r="44" ht="12.75"/>
+    <row r="45" ht="12.75"/>
+    <row r="46" ht="12.75"/>
     <row r="47" spans="3:3">
       <c r="C47" s="4"/>
     </row>
     <row r="48" spans="3:13">
       <c r="C48" s="4"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
     </row>
     <row r="49" spans="3:13">
       <c r="C49" s="4"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
     </row>
     <row r="50" spans="3:13">
       <c r="C50" s="4"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="26"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
     </row>
     <row r="51" spans="3:13">
       <c r="C51" s="4"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
     </row>
     <row r="52" ht="33" customHeight="1" spans="3:13">
       <c r="C52" s="4"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="26"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
     </row>
     <row r="53" spans="3:13">
       <c r="C53" s="4"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="26"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
     </row>
     <row r="54" spans="3:13">
       <c r="C54" s="4"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="26"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
     </row>
     <row r="55" spans="3:13">
       <c r="C55" s="4"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
     </row>
     <row r="56" spans="3:13">
       <c r="C56" s="4"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="26"/>
-      <c r="M56" s="26"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="25"/>
     </row>
     <row r="57" spans="3:13">
       <c r="C57" s="4"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="M57" s="25"/>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" s="4"/>
@@ -4040,86 +4023,86 @@
       <c r="C901" s="4"/>
     </row>
     <row r="902" ht="16.5" spans="3:3">
-      <c r="C902" s="27"/>
-    </row>
-    <row r="903"/>
-    <row r="904"/>
-    <row r="905"/>
-    <row r="906"/>
-    <row r="907"/>
-    <row r="908"/>
-    <row r="909"/>
-    <row r="910"/>
-    <row r="911"/>
-    <row r="912"/>
-    <row r="913"/>
-    <row r="914"/>
-    <row r="915"/>
-    <row r="916"/>
-    <row r="917"/>
-    <row r="918"/>
-    <row r="919"/>
-    <row r="920"/>
-    <row r="921"/>
-    <row r="922"/>
-    <row r="923"/>
-    <row r="924"/>
-    <row r="925"/>
-    <row r="926"/>
-    <row r="927"/>
-    <row r="928"/>
-    <row r="929"/>
-    <row r="930"/>
-    <row r="931"/>
-    <row r="932"/>
-    <row r="933"/>
-    <row r="934"/>
-    <row r="935"/>
-    <row r="936"/>
-    <row r="937"/>
-    <row r="938"/>
-    <row r="939"/>
-    <row r="940"/>
-    <row r="941"/>
-    <row r="942"/>
-    <row r="943"/>
-    <row r="944"/>
-    <row r="945"/>
-    <row r="946"/>
-    <row r="947"/>
-    <row r="948"/>
-    <row r="949"/>
-    <row r="950"/>
-    <row r="951"/>
-    <row r="952"/>
-    <row r="953"/>
-    <row r="954"/>
-    <row r="955"/>
-    <row r="956"/>
-    <row r="957"/>
-    <row r="958"/>
-    <row r="959"/>
-    <row r="960"/>
-    <row r="961"/>
-    <row r="962"/>
-    <row r="963"/>
-    <row r="964"/>
-    <row r="965"/>
-    <row r="966"/>
-    <row r="967"/>
-    <row r="968"/>
-    <row r="969"/>
-    <row r="970"/>
-    <row r="971"/>
-    <row r="972"/>
-    <row r="973"/>
-    <row r="974"/>
-    <row r="975"/>
-    <row r="976"/>
-    <row r="977"/>
-    <row r="978"/>
-    <row r="979"/>
-    <row r="980"/>
+      <c r="C902" s="26"/>
+    </row>
+    <row r="903" ht="13.5"/>
+    <row r="904" ht="12.75"/>
+    <row r="905" ht="12.75"/>
+    <row r="906" ht="12.75"/>
+    <row r="907" ht="12.75"/>
+    <row r="908" ht="12.75"/>
+    <row r="909" ht="12.75"/>
+    <row r="910" ht="12.75"/>
+    <row r="911" ht="12.75"/>
+    <row r="912" ht="12.75"/>
+    <row r="913" ht="12.75"/>
+    <row r="914" ht="12.75"/>
+    <row r="915" ht="12.75"/>
+    <row r="916" ht="12.75"/>
+    <row r="917" ht="12.75"/>
+    <row r="918" ht="12.75"/>
+    <row r="919" ht="12.75"/>
+    <row r="920" ht="12.75"/>
+    <row r="921" ht="12.75"/>
+    <row r="922" ht="12.75"/>
+    <row r="923" ht="12.75"/>
+    <row r="924" ht="12.75"/>
+    <row r="925" ht="12.75"/>
+    <row r="926" ht="12.75"/>
+    <row r="927" ht="12.75"/>
+    <row r="928" ht="12.75"/>
+    <row r="929" ht="12.75"/>
+    <row r="930" ht="12.75"/>
+    <row r="931" ht="12.75"/>
+    <row r="932" ht="12.75"/>
+    <row r="933" ht="12.75"/>
+    <row r="934" ht="12.75"/>
+    <row r="935" ht="12.75"/>
+    <row r="936" ht="12.75"/>
+    <row r="937" ht="12.75"/>
+    <row r="938" ht="12.75"/>
+    <row r="939" ht="12.75"/>
+    <row r="940" ht="12.75"/>
+    <row r="941" ht="12.75"/>
+    <row r="942" ht="12.75"/>
+    <row r="943" ht="12.75"/>
+    <row r="944" ht="12.75"/>
+    <row r="945" ht="12.75"/>
+    <row r="946" ht="12.75"/>
+    <row r="947" ht="12.75"/>
+    <row r="948" ht="12.75"/>
+    <row r="949" ht="12.75"/>
+    <row r="950" ht="12.75"/>
+    <row r="951" ht="12.75"/>
+    <row r="952" ht="12.75"/>
+    <row r="953" ht="12.75"/>
+    <row r="954" ht="12.75"/>
+    <row r="955" ht="12.75"/>
+    <row r="956" ht="12.75"/>
+    <row r="957" ht="12.75"/>
+    <row r="958" ht="12.75"/>
+    <row r="959" ht="12.75"/>
+    <row r="960" ht="12.75"/>
+    <row r="961" ht="12.75"/>
+    <row r="962" ht="12.75"/>
+    <row r="963" ht="12.75"/>
+    <row r="964" ht="12.75"/>
+    <row r="965" ht="12.75"/>
+    <row r="966" ht="12.75"/>
+    <row r="967" ht="12.75"/>
+    <row r="968" ht="12.75"/>
+    <row r="969" ht="12.75"/>
+    <row r="970" ht="12.75"/>
+    <row r="971" ht="12.75"/>
+    <row r="972" ht="12.75"/>
+    <row r="973" ht="12.75"/>
+    <row r="974" ht="12.75"/>
+    <row r="975" ht="12.75"/>
+    <row r="976" ht="12.75"/>
+    <row r="977" ht="12.75"/>
+    <row r="978" ht="12.75"/>
+    <row r="979" ht="12.75"/>
+    <row r="980" ht="12.75"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A4:A7"/>

</xml_diff>